<commit_message>
# Conclusions 48 - 4 layers - ('relu', 'relu') with batch 400 and widths 450 - Local test (not in AWS) - not exactly the same results in both - Accuracy: .983-.984, 2/3 .984 ### Conclusions going forward: - Compare to tanh, relu local 200, 200
# Conclusions 49 - 4 layers - ('relu', 'relu') with batch and widths around 450
- On AWS:
- Both 450 seems the best - test accuracy .9848. Both some are good with 400, 450, 500.  So staying in the middle
### Conclusions going forward:
- Change batch and width to 450
</commit_message>
<xml_diff>
--- a/output/47_4_layers_relu_relu_around_400_400/full.xlsx
+++ b/output/47_4_layers_relu_relu_around_400_400/full.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rkrichev\Documents\Yoni\DataScience\data-science-ml-dl-mnist\output\47_4_layers_relu_relu_around_400_400\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -82,8 +87,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,10 +140,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -146,6 +157,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -192,7 +211,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -224,9 +243,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -258,6 +278,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -433,76 +454,78 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:21">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
+    <row r="1" spans="1:21" s="3" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -519,7 +542,7 @@
         <v>350</v>
       </c>
       <c r="F2">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="G2">
         <v>17.4693</v>
@@ -540,10 +563,10 @@
         <v>1</v>
       </c>
       <c r="M2">
-        <v>0.984000027179718</v>
+        <v>0.98400002717971802</v>
       </c>
       <c r="N2">
-        <v>0.08119999999999999</v>
+        <v>8.1199999999999994E-2</v>
       </c>
       <c r="O2">
         <v>1</v>
@@ -552,7 +575,7 @@
         <v>0</v>
       </c>
       <c r="Q2">
-        <v>215.139</v>
+        <v>215.13900000000001</v>
       </c>
       <c r="R2">
         <v>1</v>
@@ -561,18 +584,18 @@
         <v>0</v>
       </c>
       <c r="T2">
-        <v>0.0001</v>
+        <v>1E-4</v>
       </c>
       <c r="U2">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>5.6123</v>
+        <v>5.6123000000000003</v>
       </c>
       <c r="C3">
         <v>350</v>
@@ -584,7 +607,7 @@
         <v>400</v>
       </c>
       <c r="F3">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="G3">
         <v>14.693</v>
@@ -605,39 +628,39 @@
         <v>1</v>
       </c>
       <c r="M3">
-        <v>0.984499990940094</v>
+        <v>0.98449999094009399</v>
       </c>
       <c r="N3">
-        <v>0.077</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="O3">
-        <v>0.9980999827384949</v>
+        <v>0.99809998273849487</v>
       </c>
       <c r="P3">
-        <v>0.0059</v>
+        <v>5.8999999999999999E-3</v>
       </c>
       <c r="Q3">
-        <v>190.819</v>
+        <v>190.81899999999999</v>
       </c>
       <c r="R3">
-        <v>0.9976999759674072</v>
+        <v>0.99769997596740723</v>
       </c>
       <c r="S3">
-        <v>0.007</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="T3">
-        <v>0.0001</v>
+        <v>1E-4</v>
       </c>
       <c r="U3">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>5.7326</v>
+        <v>5.7325999999999997</v>
       </c>
       <c r="C4">
         <v>350</v>
@@ -649,10 +672,10 @@
         <v>450</v>
       </c>
       <c r="F4">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="G4">
-        <v>14.2901</v>
+        <v>14.290100000000001</v>
       </c>
       <c r="H4">
         <v>1000</v>
@@ -670,19 +693,19 @@
         <v>1</v>
       </c>
       <c r="M4">
-        <v>0.9842000007629395</v>
+        <v>0.98420000076293945</v>
       </c>
       <c r="N4">
-        <v>0.0779</v>
+        <v>7.7899999999999997E-2</v>
       </c>
       <c r="O4">
         <v>1</v>
       </c>
       <c r="P4">
-        <v>0.0003</v>
+        <v>2.9999999999999997E-4</v>
       </c>
       <c r="Q4">
-        <v>183.442</v>
+        <v>183.44200000000001</v>
       </c>
       <c r="R4">
         <v>1</v>
@@ -691,18 +714,18 @@
         <v>0</v>
       </c>
       <c r="T4">
-        <v>0.0001</v>
+        <v>1E-4</v>
       </c>
       <c r="U4">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>5.3906</v>
+        <v>5.3906000000000001</v>
       </c>
       <c r="C5">
         <v>400</v>
@@ -714,10 +737,10 @@
         <v>350</v>
       </c>
       <c r="F5">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="G5">
-        <v>18.1576</v>
+        <v>18.157599999999999</v>
       </c>
       <c r="H5">
         <v>1000</v>
@@ -735,10 +758,10 @@
         <v>1</v>
       </c>
       <c r="M5">
-        <v>0.9843000173568726</v>
+        <v>0.98430001735687256</v>
       </c>
       <c r="N5">
-        <v>0.08019999999999999</v>
+        <v>8.0199999999999994E-2</v>
       </c>
       <c r="O5">
         <v>1</v>
@@ -756,18 +779,18 @@
         <v>0</v>
       </c>
       <c r="T5">
-        <v>0.0001</v>
+        <v>1E-4</v>
       </c>
       <c r="U5">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>5.4876</v>
+        <v>5.4875999999999996</v>
       </c>
       <c r="C6">
         <v>400</v>
@@ -779,10 +802,10 @@
         <v>400</v>
       </c>
       <c r="F6">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="G6">
-        <v>9.601100000000001</v>
+        <v>9.6011000000000006</v>
       </c>
       <c r="H6">
         <v>1000</v>
@@ -800,39 +823,39 @@
         <v>1</v>
       </c>
       <c r="M6">
-        <v>0.982699990272522</v>
+        <v>0.98269999027252197</v>
       </c>
       <c r="N6">
-        <v>0.07290000000000001</v>
+        <v>7.2900000000000006E-2</v>
       </c>
       <c r="O6">
-        <v>0.9991999864578247</v>
+        <v>0.99919998645782471</v>
       </c>
       <c r="P6">
-        <v>0.0027</v>
+        <v>2.7000000000000001E-3</v>
       </c>
       <c r="Q6">
         <v>131.702</v>
       </c>
       <c r="R6">
-        <v>0.9976999759674072</v>
+        <v>0.99769997596740723</v>
       </c>
       <c r="S6">
-        <v>0.0072</v>
+        <v>7.1999999999999998E-3</v>
       </c>
       <c r="T6">
-        <v>0.0001</v>
+        <v>1E-4</v>
       </c>
       <c r="U6">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>5.6284</v>
+        <v>5.6284000000000001</v>
       </c>
       <c r="C7">
         <v>400</v>
@@ -844,10 +867,10 @@
         <v>450</v>
       </c>
       <c r="F7">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="G7">
-        <v>21.348</v>
+        <v>21.347999999999999</v>
       </c>
       <c r="H7">
         <v>1000</v>
@@ -865,10 +888,10 @@
         <v>1</v>
       </c>
       <c r="M7">
-        <v>0.9847999811172485</v>
+        <v>0.98479998111724854</v>
       </c>
       <c r="N7">
-        <v>0.08069999999999999</v>
+        <v>8.0699999999999994E-2</v>
       </c>
       <c r="O7">
         <v>1</v>
@@ -886,18 +909,18 @@
         <v>0</v>
       </c>
       <c r="T7">
-        <v>0.0001</v>
+        <v>1E-4</v>
       </c>
       <c r="U7">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>5.3429</v>
+        <v>5.3429000000000002</v>
       </c>
       <c r="C8">
         <v>450</v>
@@ -909,7 +932,7 @@
         <v>350</v>
       </c>
       <c r="F8">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="G8">
         <v>17.8094</v>
@@ -930,10 +953,10 @@
         <v>1</v>
       </c>
       <c r="M8">
-        <v>0.9829999804496765</v>
+        <v>0.98299998044967651</v>
       </c>
       <c r="N8">
-        <v>0.0813</v>
+        <v>8.1299999999999997E-2</v>
       </c>
       <c r="O8">
         <v>1</v>
@@ -942,7 +965,7 @@
         <v>0</v>
       </c>
       <c r="Q8">
-        <v>219.058</v>
+        <v>219.05799999999999</v>
       </c>
       <c r="R8">
         <v>1</v>
@@ -951,18 +974,18 @@
         <v>0</v>
       </c>
       <c r="T8">
-        <v>0.0001</v>
+        <v>1E-4</v>
       </c>
       <c r="U8">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>5.4462</v>
+        <v>5.4462000000000002</v>
       </c>
       <c r="C9">
         <v>450</v>
@@ -974,10 +997,10 @@
         <v>400</v>
       </c>
       <c r="F9">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="G9">
-        <v>18.969</v>
+        <v>18.969000000000001</v>
       </c>
       <c r="H9">
         <v>1000</v>
@@ -995,16 +1018,16 @@
         <v>1</v>
       </c>
       <c r="M9">
-        <v>0.9840999841690063</v>
+        <v>0.98409998416900635</v>
       </c>
       <c r="N9">
-        <v>0.081</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="O9">
         <v>1</v>
       </c>
       <c r="P9">
-        <v>0.0003</v>
+        <v>2.9999999999999997E-4</v>
       </c>
       <c r="Q9">
         <v>234.185</v>
@@ -1016,18 +1039,18 @@
         <v>0</v>
       </c>
       <c r="T9">
-        <v>0.0001</v>
+        <v>1E-4</v>
       </c>
       <c r="U9">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>5.5896</v>
+        <v>5.5895999999999999</v>
       </c>
       <c r="C10">
         <v>450</v>
@@ -1039,7 +1062,7 @@
         <v>450</v>
       </c>
       <c r="F10">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="G10">
         <v>24.4268</v>
@@ -1060,10 +1083,10 @@
         <v>1</v>
       </c>
       <c r="M10">
-        <v>0.9843000173568726</v>
+        <v>0.98430001735687256</v>
       </c>
       <c r="N10">
-        <v>0.08740000000000001</v>
+        <v>8.7400000000000005E-2</v>
       </c>
       <c r="O10">
         <v>1</v>
@@ -1072,7 +1095,7 @@
         <v>0</v>
       </c>
       <c r="Q10">
-        <v>279.482</v>
+        <v>279.48200000000003</v>
       </c>
       <c r="R10">
         <v>1</v>
@@ -1081,13 +1104,38 @@
         <v>0</v>
       </c>
       <c r="T10">
-        <v>0.0001</v>
+        <v>1E-4</v>
       </c>
       <c r="U10">
         <v>10</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="M2:M10">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G10">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>